<commit_message>
Calibrated for scene 3
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tom\Desktop\thesisWindows\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F1D6E97-A16C-435C-A10F-BD6F055CBF42}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD9B7F8-80C4-4C43-9F84-AC7B4DD051E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{5472FFC1-A34E-4083-9BA3-0CA3CBEE0BD9}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{5472FFC1-A34E-4083-9BA3-0CA3CBEE0BD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Location 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="46">
   <si>
     <t>Lane</t>
   </si>
@@ -134,6 +134,45 @@
   </si>
   <si>
     <t>Location: 3 (45 seconds)</t>
+  </si>
+  <si>
+    <t>R3/R4</t>
+  </si>
+  <si>
+    <t>Merged two SUVs</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R32/R3</t>
+  </si>
+  <si>
+    <t>Car same color as road</t>
+  </si>
+  <si>
+    <t>Sedan &amp; SUV merge</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>Because camera is moving slightly while filming the road causing lane to make a blob with a moving centroid (Down)</t>
+  </si>
+  <si>
+    <t>Because camera is moving slightly while filming the road causing lane to make a blob with a moving centroid (Up)</t>
+  </si>
+  <si>
+    <t>Two SUVs Merge</t>
+  </si>
+  <si>
+    <t>Truck and Sedan Merge</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>Anomolous blob from camera moving jumps across the line and reads. (Down)</t>
   </si>
 </sst>
 </file>
@@ -198,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -218,8 +257,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -227,14 +269,14 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -553,7 +595,7 @@
   <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,24 +606,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="M1" s="10" t="s">
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="M1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
       <c r="R1" s="2"/>
@@ -621,11 +663,11 @@
       <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -672,7 +714,7 @@
       <c r="N3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -721,7 +763,7 @@
       <c r="N4" s="1">
         <v>480</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="9" t="s">
         <v>29</v>
       </c>
     </row>
@@ -773,7 +815,7 @@
       <c r="N5" s="1">
         <v>780</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="9" t="s">
         <v>30</v>
       </c>
     </row>
@@ -785,7 +827,7 @@
       <c r="N6" s="1">
         <v>830</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="9" t="s">
         <v>31</v>
       </c>
     </row>
@@ -793,15 +835,15 @@
       <c r="L7" s="2"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-      <c r="O7" s="12"/>
+      <c r="O7" s="9"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L8" s="2"/>
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L9" s="2"/>
@@ -811,7 +853,7 @@
       <c r="N9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -837,7 +879,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D46B6B6-5DB8-42CA-B901-955D330587E6}">
   <dimension ref="A1:O10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -848,24 +890,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="14"/>
-      <c r="M1" s="10" t="s">
+      <c r="M1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -901,11 +943,11 @@
       <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="11" t="s">
+      <c r="M2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -947,7 +989,7 @@
       <c r="N3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="13" t="s">
+      <c r="O3" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -993,7 +1035,7 @@
       <c r="N4" s="1">
         <v>863</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="9" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1004,7 +1046,7 @@
       <c r="N5" s="1">
         <v>1080</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="9" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1015,7 +1057,7 @@
       <c r="N6" s="1">
         <v>1168</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="9" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1026,16 +1068,16 @@
       <c r="N7" s="1">
         <v>1198</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="9" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M8" s="11" t="s">
+      <c r="M8" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M9" s="5" t="s">
@@ -1044,7 +1086,7 @@
       <c r="N9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1055,7 +1097,7 @@
       <c r="N10" s="1">
         <v>914</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="9" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1072,37 +1114,33 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E7195F4-5D4C-46BF-95AD-D8D6A82FAE6C}">
-  <dimension ref="A1:O10"/>
+  <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="12.5703125" customWidth="1"/>
-    <col min="15" max="15" width="60.7109375" customWidth="1"/>
+    <col min="15" max="15" width="78.85546875" customWidth="1"/>
+    <col min="18" max="18" width="75.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
       <c r="K1" s="14"/>
-      <c r="M1" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
@@ -1138,122 +1176,137 @@
       <c r="K2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>38</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1">
-        <v>42</v>
-      </c>
-      <c r="H3" s="7" t="e">
+      <c r="F3" s="1">
+        <f>D3+B3</f>
+        <v>39</v>
+      </c>
+      <c r="G3" s="5">
+        <v>41</v>
+      </c>
+      <c r="H3" s="7">
         <f>D3/(D3+B3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I3" s="7" t="e">
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="I3" s="7">
         <f>D3/(D3+C3)</f>
-        <v>#DIV/0!</v>
+        <v>0.92682926829268297</v>
       </c>
       <c r="J3" s="8">
         <f>(D3+E3)/G3</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="8" t="e">
+        <v>0.92682926829268297</v>
+      </c>
+      <c r="K3" s="8">
         <f>2*(1/((1/H3)+(1/I3)))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="O3" s="13" t="s">
-        <v>18</v>
+        <v>0.94999999999999984</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>38</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1">
+      <c r="F4" s="1">
+        <v>40</v>
+      </c>
+      <c r="G4" s="5">
         <v>39</v>
       </c>
-      <c r="H4" s="7" t="e">
+      <c r="H4" s="7">
         <f>D4/(D4+B4)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I4" s="7" t="e">
+        <v>0.95</v>
+      </c>
+      <c r="I4" s="7">
         <f>D4/(D4+C4)</f>
-        <v>#DIV/0!</v>
+        <v>0.95</v>
       </c>
       <c r="J4" s="8">
         <f>(D4+E4)/G4</f>
-        <v>0</v>
-      </c>
-      <c r="K4" s="8" t="e">
+        <v>0.97435897435897434</v>
+      </c>
+      <c r="K4" s="8">
         <f>2*(1/((1/H4)+(1/I4)))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="12"/>
+        <v>0.95000000000000007</v>
+      </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="7" t="e">
+      <c r="B5" s="1">
+        <f>SUM(B3:B4)</f>
+        <v>3</v>
+      </c>
+      <c r="C5" s="1">
+        <f>SUM(C3:C4)</f>
+        <v>5</v>
+      </c>
+      <c r="D5" s="1">
+        <f>SUM(D3:D4)</f>
+        <v>76</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <f t="shared" ref="F4:F5" si="0">D5+B5</f>
+        <v>79</v>
+      </c>
+      <c r="G5" s="5">
+        <f>SUM(G3:G4)</f>
+        <v>80</v>
+      </c>
+      <c r="H5" s="7">
         <f>D5/(D5+B5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="I5" s="7" t="e">
+        <v>0.96202531645569622</v>
+      </c>
+      <c r="I5" s="7">
         <f>D5/(D5+C5)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="J5" s="8" t="e">
+        <v>0.93827160493827155</v>
+      </c>
+      <c r="J5" s="8">
         <f>(D5+E5)/G5</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="K5" s="8" t="e">
+        <v>0.95</v>
+      </c>
+      <c r="K5" s="8">
         <f>2*(1/((1/H5)+(1/I5)))</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="12"/>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="12"/>
+        <v>0.94999999999999984</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="12"/>
+      <c r="M7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
+      <c r="M8" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="12"/>
+      <c r="O8" s="12"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="M9" s="5" t="s">
@@ -1262,22 +1315,125 @@
       <c r="N9" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O9" s="13" t="s">
+      <c r="O9" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="12"/>
+      <c r="M10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="N10" s="1">
+        <v>650</v>
+      </c>
+      <c r="O10" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N11" s="1">
+        <v>800</v>
+      </c>
+      <c r="O11" s="9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="N12" s="1">
+        <v>920</v>
+      </c>
+      <c r="O12" s="9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M13" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="1">
+        <v>150</v>
+      </c>
+      <c r="O13" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M14" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N14" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M16" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+    </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="10" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="M18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N18" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O18" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="19" spans="13:15" ht="30" x14ac:dyDescent="0.25">
+      <c r="M19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N19" s="1">
+        <v>1000</v>
+      </c>
+      <c r="O19" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>44</v>
+      </c>
+      <c r="N20">
+        <v>1150</v>
+      </c>
+      <c r="O20" t="s">
+        <v>45</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="M1:O1"/>
-    <mergeCell ref="M2:O2"/>
     <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M16:O16"/>
+    <mergeCell ref="M7:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>